<commit_message>
Added new examples/ tweaked readme
</commit_message>
<xml_diff>
--- a/examples/CreateChartExample.xlsx
+++ b/examples/CreateChartExample.xlsx
@@ -427,34 +427,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>8.837375396787754</c:v>
+                  <c:v>8.252643144094897</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.7271193118825925</c:v>
+                  <c:v>6.68588770720516</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.050018877477071</c:v>
+                  <c:v>5.863923788494891</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.657495025471866</c:v>
+                  <c:v>0.976589030820818</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.083511191696787</c:v>
+                  <c:v>6.713361507575395</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.347005958038467</c:v>
+                  <c:v>0.5099811919552821</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.3833107503686928</c:v>
+                  <c:v>2.891980130967887</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.05319788249747659</c:v>
+                  <c:v>9.495778467361443</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.829913771517538</c:v>
+                  <c:v>9.735840553392082</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.11385672163971</c:v>
+                  <c:v>4.223498224820437</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -517,34 +517,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>17.67475079357551</c:v>
+                  <c:v>16.50528628818979</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.454238623765185</c:v>
+                  <c:v>13.37177541441032</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.100037754954143</c:v>
+                  <c:v>11.72784757698978</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.314990050943733</c:v>
+                  <c:v>1.953178061641636</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.167022383393574</c:v>
+                  <c:v>13.42672301515079</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.69401191607693</c:v>
+                  <c:v>1.019962383910564</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.7666215007373856</c:v>
+                  <c:v>5.783960261935775</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.1063957649949532</c:v>
+                  <c:v>18.99155693472289</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.659827543035076</c:v>
+                  <c:v>19.47168110678416</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16.22771344327942</c:v>
+                  <c:v>8.446996449640874</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1069,19 +1069,19 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>8.837375396787754</v>
+        <v>8.252643144094897</v>
       </c>
       <c r="C2">
-        <v>0.5085210235409798</v>
+        <v>5.405017945584013</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>17.67475079357551</v>
+        <v>16.50528628818979</v>
       </c>
       <c r="G2">
-        <v>1.01704204708196</v>
+        <v>10.81003589116803</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1089,19 +1089,19 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.7271193118825925</v>
+        <v>6.68588770720516</v>
       </c>
       <c r="C3">
-        <v>0.3690508165012485</v>
+        <v>9.925574752198022</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
       </c>
       <c r="F3">
-        <v>1.454238623765185</v>
+        <v>13.37177541441032</v>
       </c>
       <c r="G3">
-        <v>0.738101633002497</v>
+        <v>19.85114950439604</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1109,19 +1109,19 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1.050018877477071</v>
+        <v>5.863923788494891</v>
       </c>
       <c r="C4">
-        <v>4.65857261671669</v>
+        <v>3.189183188888812</v>
       </c>
       <c r="E4" s="1">
         <v>2</v>
       </c>
       <c r="F4">
-        <v>2.100037754954143</v>
+        <v>11.72784757698978</v>
       </c>
       <c r="G4">
-        <v>9.317145233433379</v>
+        <v>6.378366377777624</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1129,19 +1129,19 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>3.657495025471866</v>
+        <v>0.976589030820818</v>
       </c>
       <c r="C5">
-        <v>2.547622341388292</v>
+        <v>3.171506025267213</v>
       </c>
       <c r="E5" s="1">
         <v>3</v>
       </c>
       <c r="F5">
-        <v>7.314990050943733</v>
+        <v>1.953178061641636</v>
       </c>
       <c r="G5">
-        <v>5.095244682776585</v>
+        <v>6.343012050534426</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1149,19 +1149,19 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>4.083511191696787</v>
+        <v>6.713361507575395</v>
       </c>
       <c r="C6">
-        <v>9.953610407829043</v>
+        <v>2.976258459102171</v>
       </c>
       <c r="E6" s="1">
         <v>4</v>
       </c>
       <c r="F6">
-        <v>8.167022383393574</v>
+        <v>13.42672301515079</v>
       </c>
       <c r="G6">
-        <v>19.90722081565809</v>
+        <v>5.952516918204342</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1169,19 +1169,19 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>5.347005958038467</v>
+        <v>0.5099811919552821</v>
       </c>
       <c r="C7">
-        <v>8.739250224005314</v>
+        <v>0.01742846552266974</v>
       </c>
       <c r="E7" s="1">
         <v>5</v>
       </c>
       <c r="F7">
-        <v>10.69401191607693</v>
+        <v>1.019962383910564</v>
       </c>
       <c r="G7">
-        <v>17.47850044801063</v>
+        <v>0.03485693104533949</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1189,19 +1189,19 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.3833107503686928</v>
+        <v>2.891980130967887</v>
       </c>
       <c r="C8">
-        <v>1.116680432117803</v>
+        <v>8.653387117681449</v>
       </c>
       <c r="E8" s="1">
         <v>6</v>
       </c>
       <c r="F8">
-        <v>0.7666215007373856</v>
+        <v>5.783960261935775</v>
       </c>
       <c r="G8">
-        <v>2.233360864235605</v>
+        <v>17.3067742353629</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1209,19 +1209,19 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.05319788249747659</v>
+        <v>9.495778467361443</v>
       </c>
       <c r="C9">
-        <v>8.455868352194392</v>
+        <v>9.931725249980042</v>
       </c>
       <c r="E9" s="1">
         <v>7</v>
       </c>
       <c r="F9">
-        <v>0.1063957649949532</v>
+        <v>18.99155693472289</v>
       </c>
       <c r="G9">
-        <v>16.91173670438878</v>
+        <v>19.86345049996008</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1229,19 +1229,19 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>2.829913771517538</v>
+        <v>9.735840553392082</v>
       </c>
       <c r="C10">
-        <v>6.090882931078225</v>
+        <v>6.241923081743693</v>
       </c>
       <c r="E10" s="1">
         <v>8</v>
       </c>
       <c r="F10">
-        <v>5.659827543035076</v>
+        <v>19.47168110678416</v>
       </c>
       <c r="G10">
-        <v>12.18176586215645</v>
+        <v>12.48384616348739</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1249,19 +1249,19 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>8.11385672163971</v>
+        <v>4.223498224820437</v>
       </c>
       <c r="C11">
-        <v>9.450386262209836</v>
+        <v>8.485493146619246</v>
       </c>
       <c r="E11" s="1">
         <v>9</v>
       </c>
       <c r="F11">
-        <v>16.22771344327942</v>
+        <v>8.446996449640874</v>
       </c>
       <c r="G11">
-        <v>18.90077252441967</v>
+        <v>16.97098629323849</v>
       </c>
     </row>
   </sheetData>

</xml_diff>